<commit_message>
Mission file parsing works, needs tests.
</commit_message>
<xml_diff>
--- a/src/inits/missionfile_FF_v0.xlsx
+++ b/src/inits/missionfile_FF_v0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Cyclone Robosub\SimulinkPlant\src\inits\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FDC752-8C81-400D-92E5-AF08E175EBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9505D46C-26DD-42F4-9E68-70DC735A21BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -381,7 +381,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +415,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -426,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -437,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -448,7 +448,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -459,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>